<commit_message>
Working App V2. -Added more columns to the employees. -Made the treeview Dynamic.
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -1,51 +1,94 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radia\OneDrive\Bureau\PyProjects\Petromag\Systeme-de-pointage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E2BC64-3CF1-4DA9-9873-E78E9413C1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B4A30-A538-4AD3-81E1-49DA20029106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Matricule</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
     <t>ZENDEV</t>
   </si>
   <si>
     <t>BLAL</t>
   </si>
   <si>
-    <t>developpeur</t>
-  </si>
-  <si>
     <t>Operateur produit</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
+    <t>Fonction</t>
+  </si>
+  <si>
+    <t>Adresse</t>
+  </si>
+  <si>
+    <t>Date Recrut</t>
+  </si>
+  <si>
+    <t>Date Detach</t>
+  </si>
+  <si>
+    <t>Affect Origine</t>
+  </si>
+  <si>
+    <t>Sit Fam</t>
+  </si>
+  <si>
+    <t>Nbrs Enfants</t>
+  </si>
+  <si>
+    <t>Mustapha</t>
+  </si>
+  <si>
+    <t>Zoubir</t>
+  </si>
+  <si>
+    <t>Developpeur</t>
+  </si>
+  <si>
+    <t>veuf</t>
+  </si>
+  <si>
+    <t>Douera</t>
   </si>
 </sst>
 </file>
@@ -81,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,49 +407,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>224</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45332</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
         <v>5</v>
       </c>
     </row>

</xml_diff>